<commit_message>
ajout col somme T3
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Juin</t>
+  </si>
+  <si>
+    <t>2020 T3</t>
   </si>
   <si>
     <t>FACTURATION
@@ -526,7 +529,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -538,17 +541,17 @@
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -556,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -608,14 +611,17 @@
       <c r="S6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="T6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="6" t="s">
@@ -656,24 +662,27 @@
       <c r="R7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="U7" s="5"/>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="S7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" s="4"/>
+      <c r="U7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="11">
         <v>0</v>
@@ -715,28 +724,32 @@
       <c r="R8" s="13">
         <v>0</v>
       </c>
-      <c r="S8" s="13"/>
-      <c r="T8" s="9">
+      <c r="S8" s="8">
+        <f>P8+Q8+R8</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="13"/>
+      <c r="U8" s="9">
         <f>I8+N8+P8</f>
         <v>0</v>
       </c>
-      <c r="U8" s="9">
+      <c r="V8" s="9">
         <f>J8+O8+S8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" s="1">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="E9" s="11">
         <v>0</v>
@@ -778,28 +791,32 @@
       <c r="R9" s="13">
         <v>0</v>
       </c>
-      <c r="S9" s="13"/>
-      <c r="T9" s="9">
+      <c r="S9" s="8">
+        <f>P9+Q9+R9</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="9">
         <f>I9+N9+P9</f>
         <v>0</v>
       </c>
-      <c r="U9" s="9">
+      <c r="V9" s="9">
         <f>J9+O9+S9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22">
       <c r="A10" s="1">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="11">
         <v>0</v>
@@ -841,28 +858,32 @@
       <c r="R10" s="13">
         <v>0</v>
       </c>
-      <c r="S10" s="13"/>
-      <c r="T10" s="9">
+      <c r="S10" s="8">
+        <f>P10+Q10+R10</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="13"/>
+      <c r="U10" s="9">
         <f>I10+N10+P10</f>
         <v>0</v>
       </c>
-      <c r="U10" s="9">
+      <c r="V10" s="9">
         <f>J10+O10+S10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="11">
         <v>0</v>
@@ -904,28 +925,32 @@
       <c r="R11" s="13">
         <v>0</v>
       </c>
-      <c r="S11" s="13"/>
-      <c r="T11" s="9">
+      <c r="S11" s="8">
+        <f>P11+Q11+R11</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="13"/>
+      <c r="U11" s="9">
         <f>I11+N11+P11</f>
         <v>0</v>
       </c>
-      <c r="U11" s="9">
+      <c r="V11" s="9">
         <f>J11+O11+S11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22">
       <c r="A12" s="1">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="11">
         <v>0</v>
@@ -967,28 +992,32 @@
       <c r="R12" s="13">
         <v>0</v>
       </c>
-      <c r="S12" s="13"/>
-      <c r="T12" s="9">
+      <c r="S12" s="8">
+        <f>P12+Q12+R12</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="13"/>
+      <c r="U12" s="9">
         <f>I12+N12+P12</f>
         <v>0</v>
       </c>
-      <c r="U12" s="9">
+      <c r="V12" s="9">
         <f>J12+O12+S12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13" s="1">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="11">
         <v>0</v>
@@ -1030,28 +1059,32 @@
       <c r="R13" s="13">
         <v>0</v>
       </c>
-      <c r="S13" s="13"/>
-      <c r="T13" s="9">
+      <c r="S13" s="8">
+        <f>P13+Q13+R13</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="13"/>
+      <c r="U13" s="9">
         <f>I13+N13+P13</f>
         <v>0</v>
       </c>
-      <c r="U13" s="9">
+      <c r="V13" s="9">
         <f>J13+O13+S13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22">
       <c r="A14" s="1">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="11">
         <v>0</v>
@@ -1093,28 +1126,32 @@
       <c r="R14" s="13">
         <v>0</v>
       </c>
-      <c r="S14" s="13"/>
-      <c r="T14" s="9">
+      <c r="S14" s="8">
+        <f>P14+Q14+R14</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="13"/>
+      <c r="U14" s="9">
         <f>I14+N14+P14</f>
         <v>0</v>
       </c>
-      <c r="U14" s="9">
+      <c r="V14" s="9">
         <f>J14+O14+S14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:22">
       <c r="A15" s="1">
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" s="11">
         <v>0</v>
@@ -1156,19 +1193,23 @@
       <c r="R15" s="13">
         <v>170</v>
       </c>
-      <c r="S15" s="13"/>
-      <c r="T15" s="9">
+      <c r="S15" s="8">
+        <f>P15+Q15+R15</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="13"/>
+      <c r="U15" s="9">
         <f>I15+N15+P15</f>
         <v>0</v>
       </c>
-      <c r="U15" s="9">
+      <c r="V15" s="9">
         <f>J15+O15+S15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="24" customHeight="1">
+    <row r="16" spans="1:22" ht="24" customHeight="1">
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="11"/>
@@ -1192,10 +1233,7 @@
         <f>SUM(I8:I15)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="6">
-        <f>SUM(J8:J15)</f>
-        <v>0</v>
-      </c>
+      <c r="J16" s="6"/>
       <c r="K16" s="12">
         <f>SUM(K8:K15)</f>
         <v>0</v>
@@ -1212,10 +1250,7 @@
         <f>SUM(N8:N15)</f>
         <v>0</v>
       </c>
-      <c r="O16" s="7">
-        <f>SUM(O8:O15)</f>
-        <v>0</v>
-      </c>
+      <c r="O16" s="7"/>
       <c r="P16" s="13">
         <f>SUM(P8:P15)</f>
         <v>0</v>
@@ -1232,10 +1267,11 @@
         <f>SUM(S8:S15)</f>
         <v>0</v>
       </c>
-      <c r="T16" s="14"/>
+      <c r="T16" s="8"/>
       <c r="U16" s="14"/>
-    </row>
-    <row r="17" spans="2:21" ht="24" customHeight="1">
+      <c r="V16" s="14"/>
+    </row>
+    <row r="17" spans="2:22" ht="24" customHeight="1">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1244,37 +1280,23 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="6">
-        <f> </f>
-        <v>0</v>
-      </c>
+      <c r="J17" s="6"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="7">
-        <f> </f>
-        <v>0</v>
-      </c>
+      <c r="O17" s="7"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="8">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="T17" s="9">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="U17" s="9">
-        <f> </f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21">
+      <c r="S17" s="1"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+    </row>
+    <row r="18" spans="2:22">
       <c r="B18" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1298,15 +1320,16 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="8">
+      <c r="S18" s="1"/>
+      <c r="T18" s="8">
         <f>SUM(S8:S15)</f>
         <v>0</v>
       </c>
-      <c r="T18" s="9">
+      <c r="U18" s="9">
         <f>SUM(T8:T15)</f>
         <v>0</v>
       </c>
-      <c r="U18" s="9">
+      <c r="V18" s="9">
         <f>SUM(U8:U15)</f>
         <v>0</v>
       </c>
@@ -1319,8 +1342,8 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="V6:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
calcul du nb d'heure de cours par moi
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Sept</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Oct</t>
   </si>
   <si>
@@ -87,6 +84,12 @@
   </si>
   <si>
     <t>TOTAL €</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
   <si>
     <t>Matrod Remi</t>
@@ -220,9 +223,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,98 +576,98 @@
         <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="R6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="U6" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="9" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="U7" s="5"/>
     </row>
@@ -667,13 +676,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="11">
         <v>0</v>
@@ -730,13 +739,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="E9" s="11">
         <v>0</v>
@@ -793,13 +802,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="11">
         <v>0</v>
@@ -856,13 +865,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="11">
         <v>0</v>
@@ -919,13 +928,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="11">
         <v>0</v>
@@ -982,13 +991,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="11">
         <v>0</v>
@@ -1045,13 +1054,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="11">
         <v>0</v>
@@ -1108,13 +1117,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" s="11">
         <v>0</v>
@@ -1168,7 +1177,7 @@
     </row>
     <row r="16" spans="1:21" ht="24" customHeight="1">
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="11"/>
@@ -1274,7 +1283,7 @@
     </row>
     <row r="18" spans="2:21">
       <c r="B18" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>

</xml_diff>

<commit_message>
style pour la page admin et page changer les variables
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -89,7 +89,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>28</t>
+    <t>21</t>
   </si>
   <si>
     <t>Matrod Remi</t>
@@ -657,10 +657,10 @@
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>22</v>
@@ -719,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R8" s="13">
         <v>0</v>
@@ -782,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R9" s="13">
         <v>0</v>
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R10" s="13">
         <v>0</v>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R11" s="13">
         <v>0</v>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R12" s="13">
         <v>0</v>
@@ -1034,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R13" s="13">
         <v>0</v>
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R14" s="13">
         <v>0</v>
@@ -1160,7 +1160,7 @@
         <v>170</v>
       </c>
       <c r="Q15" s="13">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R15" s="13">
         <v>170</v>

</xml_diff>

<commit_message>
ajout colonne T3 + somme pour h par trimestre et total
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Juin</t>
+  </si>
+  <si>
+    <t>2020 T3</t>
   </si>
   <si>
     <t>FACTURATION
@@ -535,7 +538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -547,17 +550,17 @@
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -565,7 +568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -614,75 +617,85 @@
       <c r="R6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="S6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="T6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="I7" s="6">
+        <f>E7+F7+G7+H7</f>
+        <v>0</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N7" s="7">
+        <f>K7+L7+M7</f>
+        <v>0</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="R7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="U7" s="5"/>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="S7" s="8">
+        <f>P7+Q7+R7</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="4"/>
+      <c r="U7" s="9">
+        <f>I7+N7+S7</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="11">
         <v>0</v>
@@ -724,28 +737,32 @@
       <c r="R8" s="13">
         <v>0</v>
       </c>
-      <c r="S8" s="13"/>
-      <c r="T8" s="9">
+      <c r="S8" s="8">
+        <f>P8+Q8+R8</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="13"/>
+      <c r="U8" s="9">
         <f>I8+N8+P8</f>
         <v>0</v>
       </c>
-      <c r="U8" s="9">
+      <c r="V8" s="9">
         <f>J8+O8+S8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" s="1">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>26</v>
       </c>
       <c r="E9" s="11">
         <v>0</v>
@@ -787,28 +804,32 @@
       <c r="R9" s="13">
         <v>0</v>
       </c>
-      <c r="S9" s="13"/>
-      <c r="T9" s="9">
+      <c r="S9" s="8">
+        <f>P9+Q9+R9</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="9">
         <f>I9+N9+P9</f>
         <v>0</v>
       </c>
-      <c r="U9" s="9">
+      <c r="V9" s="9">
         <f>J9+O9+S9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22">
       <c r="A10" s="1">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="11">
         <v>0</v>
@@ -850,28 +871,32 @@
       <c r="R10" s="13">
         <v>0</v>
       </c>
-      <c r="S10" s="13"/>
-      <c r="T10" s="9">
+      <c r="S10" s="8">
+        <f>P10+Q10+R10</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="13"/>
+      <c r="U10" s="9">
         <f>I10+N10+P10</f>
         <v>0</v>
       </c>
-      <c r="U10" s="9">
+      <c r="V10" s="9">
         <f>J10+O10+S10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="11">
         <v>0</v>
@@ -913,28 +938,32 @@
       <c r="R11" s="13">
         <v>0</v>
       </c>
-      <c r="S11" s="13"/>
-      <c r="T11" s="9">
+      <c r="S11" s="8">
+        <f>P11+Q11+R11</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="13"/>
+      <c r="U11" s="9">
         <f>I11+N11+P11</f>
         <v>0</v>
       </c>
-      <c r="U11" s="9">
+      <c r="V11" s="9">
         <f>J11+O11+S11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22">
       <c r="A12" s="1">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" s="11">
         <v>0</v>
@@ -976,28 +1005,32 @@
       <c r="R12" s="13">
         <v>0</v>
       </c>
-      <c r="S12" s="13"/>
-      <c r="T12" s="9">
+      <c r="S12" s="8">
+        <f>P12+Q12+R12</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="13"/>
+      <c r="U12" s="9">
         <f>I12+N12+P12</f>
         <v>0</v>
       </c>
-      <c r="U12" s="9">
+      <c r="V12" s="9">
         <f>J12+O12+S12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13" s="1">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="11">
         <v>0</v>
@@ -1039,28 +1072,32 @@
       <c r="R13" s="13">
         <v>0</v>
       </c>
-      <c r="S13" s="13"/>
-      <c r="T13" s="9">
+      <c r="S13" s="8">
+        <f>P13+Q13+R13</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="13"/>
+      <c r="U13" s="9">
         <f>I13+N13+P13</f>
         <v>0</v>
       </c>
-      <c r="U13" s="9">
+      <c r="V13" s="9">
         <f>J13+O13+S13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22">
       <c r="A14" s="1">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" s="11">
         <v>0</v>
@@ -1102,28 +1139,32 @@
       <c r="R14" s="13">
         <v>0</v>
       </c>
-      <c r="S14" s="13"/>
-      <c r="T14" s="9">
+      <c r="S14" s="8">
+        <f>P14+Q14+R14</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="13"/>
+      <c r="U14" s="9">
         <f>I14+N14+P14</f>
         <v>0</v>
       </c>
-      <c r="U14" s="9">
+      <c r="V14" s="9">
         <f>J14+O14+S14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:22">
       <c r="A15" s="1">
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="11">
         <v>0</v>
@@ -1165,19 +1206,23 @@
       <c r="R15" s="13">
         <v>170</v>
       </c>
-      <c r="S15" s="13"/>
-      <c r="T15" s="9">
+      <c r="S15" s="8">
+        <f>P15+Q15+R15</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="13"/>
+      <c r="U15" s="9">
         <f>I15+N15+P15</f>
         <v>0</v>
       </c>
-      <c r="U15" s="9">
+      <c r="V15" s="9">
         <f>J15+O15+S15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="24" customHeight="1">
+    <row r="16" spans="1:22" ht="24" customHeight="1">
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="11"/>
@@ -1241,10 +1286,14 @@
         <f>SUM(S8:S15)</f>
         <v>0</v>
       </c>
-      <c r="T16" s="14"/>
+      <c r="T16" s="8">
+        <f>SUM(T8:T15)</f>
+        <v>0</v>
+      </c>
       <c r="U16" s="14"/>
-    </row>
-    <row r="17" spans="2:21" ht="24" customHeight="1">
+      <c r="V16" s="14"/>
+    </row>
+    <row r="17" spans="2:22" ht="24" customHeight="1">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1268,11 +1317,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="8">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="T17" s="9">
+      <c r="T17" s="8">
         <f> </f>
         <v>0</v>
       </c>
@@ -1280,10 +1325,14 @@
         <f> </f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:21">
+      <c r="V17" s="9">
+        <f> </f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22">
       <c r="B18" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1307,16 +1356,16 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="8">
-        <f>SUM(S8:S15)</f>
-        <v>0</v>
-      </c>
-      <c r="T18" s="9">
+      <c r="T18" s="8">
         <f>SUM(T8:T15)</f>
         <v>0</v>
       </c>
       <c r="U18" s="9">
         <f>SUM(U8:U15)</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="9">
+        <f>SUM(V8:V15)</f>
         <v>0</v>
       </c>
     </row>
@@ -1328,8 +1377,8 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="V6:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel : utilisation de la bdd administration pour récup date début / fin
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -22,7 +22,7 @@
     <t>SFC 2019/2020</t>
   </si>
   <si>
-    <t>du 09/09/2019 au 08/09/2020</t>
+    <t>du 09/09/2019 au 27/05/2020</t>
   </si>
   <si>
     <t>CP/CA</t>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>21</t>
   </si>
   <si>
     <t>Matrod Remi</t>
@@ -668,7 +665,7 @@
         <v>23</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>23</v>
@@ -689,13 +686,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E8" s="11">
         <v>0</v>
@@ -756,13 +753,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E9" s="11">
         <v>0</v>
@@ -823,13 +820,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E10" s="11">
         <v>0</v>
@@ -890,13 +887,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E11" s="11">
         <v>0</v>
@@ -957,13 +954,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E12" s="11">
         <v>0</v>
@@ -1024,13 +1021,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E13" s="11">
         <v>0</v>
@@ -1091,13 +1088,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E14" s="11">
         <v>0</v>
@@ -1158,13 +1155,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E15" s="11">
         <v>0</v>
@@ -1222,7 +1219,7 @@
     </row>
     <row r="16" spans="1:22" ht="24" customHeight="1">
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="11"/>
@@ -1332,7 +1329,7 @@
     </row>
     <row r="18" spans="2:22">
       <c r="B18" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>

</xml_diff>

<commit_message>
rupture fait avec un select + changement de contrat alt a contrat appr
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Gallet Benjamin</t>
+  </si>
+  <si>
+    <t>Petrie Eric</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Berry Rasp</t>
   </si>
   <si>
     <t>Totaux présence :</t>
@@ -132,7 +141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +153,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -208,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -239,6 +255,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -535,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1198,7 +1217,7 @@
         <v>170</v>
       </c>
       <c r="Q15" s="13">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="R15" s="13">
         <v>170</v>
@@ -1217,152 +1236,286 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="24" customHeight="1">
+    <row r="16" spans="1:22">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="E16" s="11">
-        <f>SUM(E8:E15)</f>
         <v>0</v>
       </c>
       <c r="F16" s="11">
-        <f>SUM(F8:F15)</f>
         <v>0</v>
       </c>
       <c r="G16" s="11">
-        <f>SUM(G8:G15)</f>
         <v>0</v>
       </c>
       <c r="H16" s="11">
-        <f>SUM(H8:H15)</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="11">
-        <f>SUM(I8:I15)</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
-        <f>SUM(J8:J15)</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <f>E16+F16+G16+H16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="11"/>
       <c r="K16" s="12">
-        <f>SUM(K8:K15)</f>
         <v>0</v>
       </c>
       <c r="L16" s="12">
-        <f>SUM(L8:L15)</f>
         <v>0</v>
       </c>
       <c r="M16" s="12">
-        <f>SUM(M8:M15)</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="12">
-        <f>SUM(N8:N15)</f>
-        <v>0</v>
-      </c>
-      <c r="O16" s="7">
-        <f>SUM(O8:O15)</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N16" s="7">
+        <f>K16+L16+M16</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="12"/>
       <c r="P16" s="13">
-        <f>SUM(P8:P15)</f>
         <v>0</v>
       </c>
       <c r="Q16" s="13">
-        <f>SUM(Q8:Q15)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R16" s="13">
-        <f>SUM(R8:R15)</f>
         <v>0</v>
       </c>
       <c r="S16" s="8">
-        <f>SUM(S8:S15)</f>
-        <v>0</v>
-      </c>
-      <c r="T16" s="8">
-        <f>SUM(T8:T15)</f>
-        <v>0</v>
-      </c>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-    </row>
-    <row r="17" spans="2:22" ht="24" customHeight="1">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="6">
+        <f>P16+Q16+R16</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="13"/>
+      <c r="U16" s="9">
+        <f>I16+N16+P16</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="9">
+        <f>J16+O16+S16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6">
+        <f>E17+F17+G17+H17</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0</v>
+      </c>
+      <c r="M17" s="12">
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <f>K17+L17+M17</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="12"/>
+      <c r="P17" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="13">
+        <v>7</v>
+      </c>
+      <c r="R17" s="13">
+        <v>0</v>
+      </c>
+      <c r="S17" s="8">
+        <f>P17+Q17+R17</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="13"/>
+      <c r="U17" s="9">
+        <f>I17+N17+P17</f>
+        <v>0</v>
+      </c>
+      <c r="V17" s="9">
+        <f>J17+O17+S17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="24" customHeight="1">
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11">
+        <f>SUM(E8:E17)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <f>SUM(F8:F17)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="11">
+        <f>SUM(G8:G17)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <f>SUM(H8:H17)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="11">
+        <f>SUM(I8:I17)</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="6">
+        <f>SUM(J8:J17)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <f>SUM(K8:K17)</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <f>SUM(L8:L17)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="12">
+        <f>SUM(M8:M17)</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="12">
+        <f>SUM(N8:N17)</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="7">
+        <f>SUM(O8:O17)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="13">
+        <f>SUM(P8:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="13">
+        <f>SUM(Q8:Q17)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="13">
+        <f>SUM(R8:R17)</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="8">
+        <f>SUM(S8:S17)</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="8">
+        <f>SUM(T8:T17)</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+    </row>
+    <row r="19" spans="1:22" ht="24" customHeight="1">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="6">
         <f> </f>
         <v>0</v>
       </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="7">
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="7">
         <f> </f>
         <v>0</v>
       </c>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="T17" s="8">
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="T19" s="8">
         <f> </f>
         <v>0</v>
       </c>
-      <c r="U17" s="9">
+      <c r="U19" s="9">
         <f> </f>
         <v>0</v>
       </c>
-      <c r="V17" s="9">
+      <c r="V19" s="9">
         <f> </f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:22">
-      <c r="B18" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="6">
-        <f>SUM(J8:J15)</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="7">
-        <f>SUM(O8:O15)</f>
-        <v>0</v>
-      </c>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="T18" s="8">
-        <f>SUM(T8:T15)</f>
-        <v>0</v>
-      </c>
-      <c r="U18" s="9">
-        <f>SUM(U8:U15)</f>
-        <v>0</v>
-      </c>
-      <c r="V18" s="9">
-        <f>SUM(V8:V15)</f>
+    <row r="20" spans="1:22">
+      <c r="B20" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="6">
+        <f>SUM(J8:J17)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="7">
+        <f>SUM(O8:O17)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="T20" s="8">
+        <f>SUM(T8:T17)</f>
+        <v>0</v>
+      </c>
+      <c r="U20" s="9">
+        <f>SUM(U8:U17)</f>
+        <v>0</v>
+      </c>
+      <c r="V20" s="9">
+        <f>SUM(V8:V17)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout du bouton 'retour' dans description de l'etu
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -104,28 +104,31 @@
     <t>Jacquet Virgile</t>
   </si>
   <si>
+    <t>Bob Yves</t>
+  </si>
+  <si>
+    <t>Charles Martin</t>
+  </si>
+  <si>
+    <t>Perreux Claire</t>
+  </si>
+  <si>
+    <t>Gallet Benjamin</t>
+  </si>
+  <si>
+    <t>Chabot Philipe</t>
+  </si>
+  <si>
+    <t>Petrie Eric</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
     <t>Durand Jean</t>
   </si>
   <si>
-    <t>Bob Yves</t>
-  </si>
-  <si>
-    <t>Charles Martin</t>
-  </si>
-  <si>
-    <t>Perreux Claire</t>
-  </si>
-  <si>
     <t>Kitschminyof Stephan</t>
-  </si>
-  <si>
-    <t>Gallet Benjamin</t>
-  </si>
-  <si>
-    <t>Petrie Eric</t>
-  </si>
-  <si>
-    <t>CA</t>
   </si>
   <si>
     <t>Berry Rasp</t>
@@ -554,7 +557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -734,10 +737,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M8" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N8" s="7">
         <f>K8+L8+M8</f>
@@ -748,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="13">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="R8" s="13">
         <v>0</v>
@@ -804,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N9" s="7">
         <f>K9+L9+M9</f>
@@ -815,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="13">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="R9" s="13">
         <v>0</v>
@@ -871,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N10" s="7">
         <f>K10+L10+M10</f>
@@ -882,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="13">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="R10" s="13">
         <v>0</v>
@@ -949,7 +952,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="13">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="R11" s="13">
         <v>0</v>
@@ -1005,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N12" s="7">
         <f>K12+L12+M12</f>
@@ -1016,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="13">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="R12" s="13">
         <v>0</v>
@@ -1083,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="13">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="R13" s="13">
         <v>0</v>
@@ -1150,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="13">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="R14" s="13">
         <v>0</v>
@@ -1171,13 +1174,13 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>25</v>
+      <c r="C15" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>26</v>
@@ -1203,10 +1206,10 @@
         <v>0</v>
       </c>
       <c r="L15" s="12">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="M15" s="12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N15" s="7">
         <f>K15+L15+M15</f>
@@ -1214,13 +1217,13 @@
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="13">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="13">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="R15" s="13">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="S15" s="8">
         <f>P15+Q15+R15</f>
@@ -1238,13 +1241,13 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>26</v>
@@ -1284,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="13">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="R16" s="13">
         <v>0</v>
@@ -1305,13 +1308,13 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>26</v>
@@ -1351,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="13">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="R17" s="13">
         <v>0</v>
@@ -1370,120 +1373,148 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="24" customHeight="1">
+    <row r="18" spans="1:22">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
       <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="E18" s="11">
-        <f>SUM(E8:E17)</f>
         <v>0</v>
       </c>
       <c r="F18" s="11">
-        <f>SUM(F8:F17)</f>
         <v>0</v>
       </c>
       <c r="G18" s="11">
-        <f>SUM(G8:G17)</f>
         <v>0</v>
       </c>
       <c r="H18" s="11">
-        <f>SUM(H8:H17)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="11">
-        <f>SUM(I8:I17)</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="6">
-        <f>SUM(J8:J17)</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I18" s="6">
+        <f>E18+F18+G18+H18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="11"/>
       <c r="K18" s="12">
-        <f>SUM(K8:K17)</f>
         <v>0</v>
       </c>
       <c r="L18" s="12">
-        <f>SUM(L8:L17)</f>
         <v>0</v>
       </c>
       <c r="M18" s="12">
-        <f>SUM(M8:M17)</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="12">
-        <f>SUM(N8:N17)</f>
-        <v>0</v>
-      </c>
-      <c r="O18" s="7">
-        <f>SUM(O8:O17)</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N18" s="7">
+        <f>K18+L18+M18</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="12"/>
       <c r="P18" s="13">
-        <f>SUM(P8:P17)</f>
         <v>0</v>
       </c>
       <c r="Q18" s="13">
-        <f>SUM(Q8:Q17)</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="R18" s="13">
-        <f>SUM(R8:R17)</f>
         <v>0</v>
       </c>
       <c r="S18" s="8">
-        <f>SUM(S8:S17)</f>
-        <v>0</v>
-      </c>
-      <c r="T18" s="8">
-        <f>SUM(T8:T17)</f>
-        <v>0</v>
-      </c>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
+        <f>P18+Q18+R18</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="13"/>
+      <c r="U18" s="9">
+        <f>I18+N18+P18</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="9">
+        <f>J18+O18+S18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:22" ht="24" customHeight="1">
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11">
+        <f>SUM(E8:E18)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <f>SUM(F8:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="11">
+        <f>SUM(G8:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="11">
+        <f>SUM(H8:H18)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="11">
+        <f>SUM(I8:I18)</f>
+        <v>0</v>
+      </c>
       <c r="J19" s="6">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+        <f>SUM(J8:J18)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="12">
+        <f>SUM(K8:K18)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <f>SUM(L8:L18)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="12">
+        <f>SUM(M8:M18)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="12">
+        <f>SUM(N8:N18)</f>
+        <v>0</v>
+      </c>
       <c r="O19" s="7">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+        <f>SUM(O8:O18)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="13">
+        <f>SUM(P8:P18)</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="13">
+        <f>SUM(Q8:Q18)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="13">
+        <f>SUM(R8:R18)</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="8">
+        <f>SUM(S8:S18)</f>
+        <v>0</v>
+      </c>
       <c r="T19" s="8">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="U19" s="9">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="V19" s="9">
-        <f> </f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="B20" s="16" t="s">
-        <v>38</v>
-      </c>
+        <f>SUM(T8:T18)</f>
+        <v>0</v>
+      </c>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+    </row>
+    <row r="20" spans="1:22" ht="24" customHeight="1">
+      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1492,7 +1523,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="6">
-        <f>SUM(J8:J17)</f>
+        <f> </f>
         <v>0</v>
       </c>
       <c r="K20" s="1"/>
@@ -1500,22 +1531,61 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="7">
-        <f>SUM(O8:O17)</f>
+        <f> </f>
         <v>0</v>
       </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="T20" s="8">
-        <f>SUM(T8:T17)</f>
+        <f> </f>
         <v>0</v>
       </c>
       <c r="U20" s="9">
-        <f>SUM(U8:U17)</f>
+        <f> </f>
         <v>0</v>
       </c>
       <c r="V20" s="9">
-        <f>SUM(V8:V17)</f>
+        <f> </f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="B21" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="6">
+        <f>SUM(J8:J18)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="7">
+        <f>SUM(O8:O18)</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="T21" s="8">
+        <f>SUM(T8:T18)</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="9">
+        <f>SUM(U8:U18)</f>
+        <v>0</v>
+      </c>
+      <c r="V21" s="9">
+        <f>SUM(V8:V18)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout du changement de signature
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -19,10 +19,10 @@
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
   <si>
-    <t>SFC 2020/2020</t>
-  </si>
-  <si>
-    <t>du 01/01/2020 au 05/05/2020</t>
+    <t>SFC 2019/2020</t>
+  </si>
+  <si>
+    <t>du 16/09/2019 au 20/06/2020</t>
   </si>
   <si>
     <t>CP/CA</t>
@@ -44,7 +44,7 @@
     <t>Déc</t>
   </si>
   <si>
-    <t>2020 T1</t>
+    <t>2019 T1</t>
   </si>
   <si>
     <t>FACTURATION
@@ -1153,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="13">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="R14" s="13">
         <v>0</v>

</xml_diff>

<commit_message>
étudiant dans ordre alphabétique
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -95,13 +95,16 @@
     <t>49</t>
   </si>
   <si>
+    <t>Charles Martin</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>7500€</t>
+  </si>
+  <si>
     <t>Gallet Benjamin</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>8 500,00€</t>
   </si>
   <si>
     <t>Totaux présence :</t>
@@ -524,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="13">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="R8" s="13">
         <v>0</v>
@@ -737,120 +740,148 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="24" customHeight="1">
+    <row r="9" spans="1:22">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="11">
-        <f>SUM(E8:E8)</f>
         <v>0</v>
       </c>
       <c r="F9" s="11">
-        <f>SUM(F8:F8)</f>
         <v>0</v>
       </c>
       <c r="G9" s="11">
-        <f>SUM(G8:G8)</f>
         <v>0</v>
       </c>
       <c r="H9" s="11">
-        <f>SUM(H8:H8)</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="11">
-        <f>SUM(I8:I8)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <f>SUM(J8:J8)</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <f>E9+F9+G9+H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="11"/>
       <c r="K9" s="12">
-        <f>SUM(K8:K8)</f>
         <v>0</v>
       </c>
       <c r="L9" s="12">
-        <f>SUM(L8:L8)</f>
         <v>0</v>
       </c>
       <c r="M9" s="12">
-        <f>SUM(M8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="12">
-        <f>SUM(N8:N8)</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="7">
-        <f>SUM(O8:O8)</f>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N9" s="7">
+        <f>K9+L9+M9</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="12"/>
       <c r="P9" s="13">
-        <f>SUM(P8:P8)</f>
         <v>0</v>
       </c>
       <c r="Q9" s="13">
-        <f>SUM(Q8:Q8)</f>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="R9" s="13">
-        <f>SUM(R8:R8)</f>
         <v>0</v>
       </c>
       <c r="S9" s="8">
-        <f>SUM(S8:S8)</f>
-        <v>0</v>
-      </c>
-      <c r="T9" s="8">
-        <f>SUM(T8:T8)</f>
-        <v>0</v>
-      </c>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
+        <f>P9+Q9+R9</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="9">
+        <f>I9+N9+P9</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="9">
+        <f>J9+O9+S9</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:22" ht="24" customHeight="1">
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11">
+        <f>SUM(E8:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <f>SUM(F8:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <f>SUM(G8:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <f>SUM(H8:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <f>SUM(I8:I9)</f>
+        <v>0</v>
+      </c>
       <c r="J10" s="6">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+        <f>SUM(J8:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <f>SUM(K8:K9)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <f>SUM(L8:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <f>SUM(M8:M9)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
+        <f>SUM(N8:N9)</f>
+        <v>0</v>
+      </c>
       <c r="O10" s="7">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+        <f>SUM(O8:O9)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="13">
+        <f>SUM(P8:P9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="13">
+        <f>SUM(Q8:Q9)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="13">
+        <f>SUM(R8:R9)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="8">
+        <f>SUM(S8:S9)</f>
+        <v>0</v>
+      </c>
       <c r="T10" s="8">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="U10" s="9">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="V10" s="9">
-        <f> </f>
-        <v>0</v>
-      </c>
+        <f>SUM(T8:T9)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
     </row>
-    <row r="11" spans="1:22">
-      <c r="B11" s="15" t="s">
-        <v>29</v>
-      </c>
+    <row r="11" spans="1:22" ht="24" customHeight="1">
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -859,7 +890,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="6">
-        <f>SUM(J8:J8)</f>
+        <f> </f>
         <v>0</v>
       </c>
       <c r="K11" s="1"/>
@@ -867,22 +898,61 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="7">
-        <f>SUM(O8:O8)</f>
+        <f> </f>
         <v>0</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="T11" s="8">
-        <f>SUM(T8:T8)</f>
+        <f> </f>
         <v>0</v>
       </c>
       <c r="U11" s="9">
-        <f>SUM(U8:U8)</f>
+        <f> </f>
         <v>0</v>
       </c>
       <c r="V11" s="9">
-        <f>SUM(V8:V8)</f>
+        <f> </f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="B12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="6">
+        <f>SUM(J8:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="7">
+        <f>SUM(O8:O9)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="T12" s="8">
+        <f>SUM(T8:T9)</f>
+        <v>0</v>
+      </c>
+      <c r="U12" s="9">
+        <f>SUM(U8:U9)</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="9">
+        <f>SUM(V8:V9)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correction formule et affichage colonne S
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -732,11 +732,11 @@
       </c>
       <c r="T8" s="13"/>
       <c r="U8" s="9">
-        <f>I8+N8+P8</f>
+        <f>I8+N8+S8</f>
         <v>0</v>
       </c>
       <c r="V8" s="9">
-        <f>J8+O8+S8</f>
+        <f>J8+O8+T8</f>
         <v>0</v>
       </c>
     </row>
@@ -799,11 +799,11 @@
       </c>
       <c r="T9" s="13"/>
       <c r="U9" s="9">
-        <f>I9+N9+P9</f>
+        <f>I9+N9+S9</f>
         <v>0</v>
       </c>
       <c r="V9" s="9">
-        <f>J9+O9+S9</f>
+        <f>J9+O9+T9</f>
         <v>0</v>
       </c>
     </row>
@@ -889,33 +889,19 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="6">
-        <f> </f>
-        <v>0</v>
-      </c>
+      <c r="J11" s="6"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="7">
-        <f> </f>
-        <v>0</v>
-      </c>
+      <c r="O11" s="7"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="T11" s="8">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="U11" s="9">
-        <f> </f>
-        <v>0</v>
-      </c>
-      <c r="V11" s="9">
-        <f> </f>
-        <v>0</v>
-      </c>
+      <c r="S11" s="1"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
     </row>
     <row r="12" spans="1:22">
       <c r="B12" s="15" t="s">
@@ -943,6 +929,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
       <c r="T12" s="8">
         <f>SUM(T8:T9)</f>
         <v>0</v>

</xml_diff>

<commit_message>
génère l'excel de la filière demandé
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -93,18 +93,6 @@
   </si>
   <si>
     <t>49</t>
-  </si>
-  <si>
-    <t>Charles Martin</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>7500€</t>
-  </si>
-  <si>
-    <t>Gallet Benjamin</t>
   </si>
   <si>
     <t>Totaux présence :</t>
@@ -117,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,13 +117,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -225,9 +206,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -527,7 +505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V12"/>
+  <dimension ref="B1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -544,12 +522,12 @@
     <col min="22" max="22" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="2:22">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="2:22">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -557,7 +535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="2:22">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -619,7 +597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="2:22">
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="6" t="s">
@@ -673,273 +651,139 @@
       </c>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
+    <row r="8" spans="2:22" ht="24" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10">
+        <f>SUM(E8:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <f>SUM(F8:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <f>SUM(G8:G7)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <f>SUM(H8:H7)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
+        <f>SUM(I8:I7)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <f>SUM(J8:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="11">
+        <f>SUM(K8:K7)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
+        <f>SUM(L8:L7)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="11">
+        <f>SUM(M8:M7)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="11">
+        <f>SUM(N8:N7)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
+        <f>SUM(O8:O7)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="12">
+        <f>SUM(P8:P7)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="12">
+        <f>SUM(Q8:Q7)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="12">
+        <f>SUM(R8:R7)</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="8">
+        <f>SUM(S8:S7)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="8">
+        <f>SUM(T8:T7)</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+    </row>
+    <row r="9" spans="2:22" ht="24" customHeight="1">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10" spans="2:22">
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="11">
-        <v>0</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <f>E8+F8+G8+H8</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="12">
-        <v>0</v>
-      </c>
-      <c r="M8" s="12">
-        <v>0</v>
-      </c>
-      <c r="N8" s="7">
-        <f>K8+L8+M8</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="12"/>
-      <c r="P8" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="13">
-        <v>0</v>
-      </c>
-      <c r="R8" s="13">
-        <v>0</v>
-      </c>
-      <c r="S8" s="8">
-        <f>P8+Q8+R8</f>
-        <v>0</v>
-      </c>
-      <c r="T8" s="13"/>
-      <c r="U8" s="9">
-        <f>I8+N8+S8</f>
-        <v>0</v>
-      </c>
-      <c r="V8" s="9">
-        <f>J8+O8+T8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <f>E9+F9+G9+H9</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12">
-        <v>0</v>
-      </c>
-      <c r="L9" s="12">
-        <v>0</v>
-      </c>
-      <c r="M9" s="12">
-        <v>0</v>
-      </c>
-      <c r="N9" s="7">
-        <f>K9+L9+M9</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="12"/>
-      <c r="P9" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="13">
-        <v>95</v>
-      </c>
-      <c r="R9" s="13">
-        <v>0</v>
-      </c>
-      <c r="S9" s="8">
-        <f>P9+Q9+R9</f>
-        <v>0</v>
-      </c>
-      <c r="T9" s="13"/>
-      <c r="U9" s="9">
-        <f>I9+N9+S9</f>
-        <v>0</v>
-      </c>
-      <c r="V9" s="9">
-        <f>J9+O9+T9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="24" customHeight="1">
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11">
-        <f>SUM(E8:E9)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="11">
-        <f>SUM(F8:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="11">
-        <f>SUM(G8:G9)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
-        <f>SUM(H8:H9)</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="11">
-        <f>SUM(I8:I9)</f>
-        <v>0</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="6">
-        <f>SUM(J8:J9)</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="12">
-        <f>SUM(K8:K9)</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="12">
-        <f>SUM(L8:L9)</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="12">
-        <f>SUM(M8:M9)</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <f>SUM(N8:N9)</f>
-        <v>0</v>
-      </c>
+        <f>SUM(J8:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
       <c r="O10" s="7">
-        <f>SUM(O8:O9)</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="13">
-        <f>SUM(P8:P9)</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="13">
-        <f>SUM(Q8:Q9)</f>
-        <v>0</v>
-      </c>
-      <c r="R10" s="13">
-        <f>SUM(R8:R9)</f>
-        <v>0</v>
-      </c>
-      <c r="S10" s="8">
-        <f>SUM(S8:S9)</f>
-        <v>0</v>
-      </c>
+        <f>SUM(O8:O7)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
       <c r="T10" s="8">
-        <f>SUM(T8:T9)</f>
-        <v>0</v>
-      </c>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-    </row>
-    <row r="11" spans="1:22" ht="24" customHeight="1">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="B12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="6">
-        <f>SUM(J8:J9)</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="7">
-        <f>SUM(O8:O9)</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="8">
-        <f>SUM(T8:T9)</f>
-        <v>0</v>
-      </c>
-      <c r="U12" s="9">
-        <f>SUM(U8:U9)</f>
-        <v>0</v>
-      </c>
-      <c r="V12" s="9">
-        <f>SUM(V8:V9)</f>
+        <f>SUM(T8:T7)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="9">
+        <f>SUM(U8:U7)</f>
+        <v>0</v>
+      </c>
+      <c r="V10" s="9">
+        <f>SUM(V8:V7)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modifEtu -> un textarea pour le commentaire
</commit_message>
<xml_diff>
--- a/app/static/excel/forfaitHorraire.xlsx
+++ b/app/static/excel/forfaitHorraire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>49</t>
+  </si>
+  <si>
+    <t>Charles Martin</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>7500€</t>
+  </si>
+  <si>
+    <t>Gallet Benjamin</t>
   </si>
   <si>
     <t>Totaux présence :</t>
@@ -105,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +129,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -206,6 +225,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -505,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:V10"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,12 +544,12 @@
     <col min="22" max="22" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22">
+    <row r="1" spans="1:22">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:22">
+    <row r="3" spans="1:22">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -535,7 +557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:22">
+    <row r="6" spans="1:22">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -597,7 +619,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:22">
+    <row r="7" spans="1:22">
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="6" t="s">
@@ -651,139 +673,273 @@
       </c>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="2:22" ht="24" customHeight="1">
+    <row r="8" spans="1:22">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
-        <f>SUM(E8:E7)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="10">
-        <f>SUM(F8:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="10">
-        <f>SUM(G8:G7)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="10">
-        <f>SUM(H8:H7)</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="10">
-        <f>SUM(I8:I7)</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <f>SUM(J8:J7)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="11">
-        <f>SUM(K8:K7)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="11">
-        <f>SUM(L8:L7)</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="11">
-        <f>SUM(M8:M7)</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="11">
-        <f>SUM(N8:N7)</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="7">
-        <f>SUM(O8:O7)</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="12">
-        <f>SUM(P8:P7)</f>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="12">
-        <f>SUM(Q8:Q7)</f>
-        <v>0</v>
-      </c>
-      <c r="R8" s="12">
-        <f>SUM(R8:R7)</f>
+      <c r="C8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
+        <f>E8+F8+G8+H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
+        <f>K8+L8+M8</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="12"/>
+      <c r="P8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>0</v>
+      </c>
+      <c r="R8" s="13">
         <v>0</v>
       </c>
       <c r="S8" s="8">
-        <f>SUM(S8:S7)</f>
-        <v>0</v>
-      </c>
-      <c r="T8" s="8">
-        <f>SUM(T8:T7)</f>
-        <v>0</v>
-      </c>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
+        <f>P8+Q8+R8</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="13"/>
+      <c r="U8" s="9">
+        <f>I8+N8+S8</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="9">
+        <f>J8+O8+T8</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="2:22" ht="24" customHeight="1">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
+    <row r="9" spans="1:22">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <f>E9+F9+G9+H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="12">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
+      <c r="N9" s="7">
+        <f>K9+L9+M9</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="12"/>
+      <c r="P9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>95</v>
+      </c>
+      <c r="R9" s="13">
+        <v>0</v>
+      </c>
+      <c r="S9" s="8">
+        <f>P9+Q9+R9</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="9">
+        <f>I9+N9+S9</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="9">
+        <f>J9+O9+T9</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="2:22">
-      <c r="B10" s="14" t="s">
-        <v>26</v>
+    <row r="10" spans="1:22" ht="24" customHeight="1">
+      <c r="B10" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11">
+        <f>SUM(E8:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <f>SUM(F8:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <f>SUM(G8:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <f>SUM(H8:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <f>SUM(I8:I9)</f>
+        <v>0</v>
+      </c>
       <c r="J10" s="6">
-        <f>SUM(J8:J7)</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+        <f>SUM(J8:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <f>SUM(K8:K9)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <f>SUM(L8:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <f>SUM(M8:M9)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
+        <f>SUM(N8:N9)</f>
+        <v>0</v>
+      </c>
       <c r="O10" s="7">
-        <f>SUM(O8:O7)</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
+        <f>SUM(O8:O9)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="13">
+        <f>SUM(P8:P9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="13">
+        <f>SUM(Q8:Q9)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="13">
+        <f>SUM(R8:R9)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="8">
+        <f>SUM(S8:S9)</f>
+        <v>0</v>
+      </c>
       <c r="T10" s="8">
-        <f>SUM(T8:T7)</f>
-        <v>0</v>
-      </c>
-      <c r="U10" s="9">
-        <f>SUM(U8:U7)</f>
-        <v>0</v>
-      </c>
-      <c r="V10" s="9">
-        <f>SUM(V8:V7)</f>
+        <f>SUM(T8:T9)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+    </row>
+    <row r="11" spans="1:22" ht="24" customHeight="1">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="B12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="6">
+        <f>SUM(J8:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="7">
+        <f>SUM(O8:O9)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="8">
+        <f>SUM(T8:T9)</f>
+        <v>0</v>
+      </c>
+      <c r="U12" s="9">
+        <f>SUM(U8:U9)</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="9">
+        <f>SUM(V8:V9)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>